<commit_message>
Added new script modules
</commit_message>
<xml_diff>
--- a/ThemisAutomation/src/main/java/themis/Data/GoldThemis.xlsx
+++ b/ThemisAutomation/src/main/java/themis/Data/GoldThemis.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{43B590BE-D690-440A-B9C0-A9A36CE42DCB}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{67A06C72-7FB4-4905-AD87-48605D0DD699}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
     <workbookView activeTab="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="881">
   <si>
     <t>CustomerReference</t>
   </si>
@@ -2429,6 +2429,237 @@
   </si>
   <si>
     <t>C-106761</t>
+  </si>
+  <si>
+    <t>10-1307764</t>
+  </si>
+  <si>
+    <t>OF-222433</t>
+  </si>
+  <si>
+    <t>10-1307792</t>
+  </si>
+  <si>
+    <t>C-106767</t>
+  </si>
+  <si>
+    <t>C-117487</t>
+  </si>
+  <si>
+    <t>10-1320418</t>
+  </si>
+  <si>
+    <t>C-117502</t>
+  </si>
+  <si>
+    <t>10-1320419</t>
+  </si>
+  <si>
+    <t>C-117509</t>
+  </si>
+  <si>
+    <t>10-1320421</t>
+  </si>
+  <si>
+    <t>C-117517</t>
+  </si>
+  <si>
+    <t>10-1320424</t>
+  </si>
+  <si>
+    <t>C-117518</t>
+  </si>
+  <si>
+    <t>10-1330620</t>
+  </si>
+  <si>
+    <t>C-117523</t>
+  </si>
+  <si>
+    <t>10-1307793</t>
+  </si>
+  <si>
+    <t>C-106769</t>
+  </si>
+  <si>
+    <t>10-1307794</t>
+  </si>
+  <si>
+    <t>C-106770</t>
+  </si>
+  <si>
+    <t>10-1307795</t>
+  </si>
+  <si>
+    <t>C-106771</t>
+  </si>
+  <si>
+    <t>10-1307796</t>
+  </si>
+  <si>
+    <t>C-106772</t>
+  </si>
+  <si>
+    <t>10-1307798</t>
+  </si>
+  <si>
+    <t>C-106774</t>
+  </si>
+  <si>
+    <t>10-1330637</t>
+  </si>
+  <si>
+    <t>C-117586</t>
+  </si>
+  <si>
+    <t>10-1330628</t>
+  </si>
+  <si>
+    <t>C-117588</t>
+  </si>
+  <si>
+    <t>10-1330639</t>
+  </si>
+  <si>
+    <t>C-117590</t>
+  </si>
+  <si>
+    <t>10-1307799</t>
+  </si>
+  <si>
+    <t>C-106775</t>
+  </si>
+  <si>
+    <t>10-1307800</t>
+  </si>
+  <si>
+    <t>C-106776</t>
+  </si>
+  <si>
+    <t>10-1307801</t>
+  </si>
+  <si>
+    <t>C-106777</t>
+  </si>
+  <si>
+    <t>10-1307802</t>
+  </si>
+  <si>
+    <t>C-106778</t>
+  </si>
+  <si>
+    <t>10-1307803</t>
+  </si>
+  <si>
+    <t>C-106779</t>
+  </si>
+  <si>
+    <t>10-1307804</t>
+  </si>
+  <si>
+    <t>C-106781</t>
+  </si>
+  <si>
+    <t>10-1307805</t>
+  </si>
+  <si>
+    <t>C-106782</t>
+  </si>
+  <si>
+    <t>10-1307905</t>
+  </si>
+  <si>
+    <t>OF-222470</t>
+  </si>
+  <si>
+    <t>10-1307980</t>
+  </si>
+  <si>
+    <t>10-1307981</t>
+  </si>
+  <si>
+    <t>C-106784</t>
+  </si>
+  <si>
+    <t>10-1307985</t>
+  </si>
+  <si>
+    <t>10-1307984</t>
+  </si>
+  <si>
+    <t>C-106785</t>
+  </si>
+  <si>
+    <t>10-1307986</t>
+  </si>
+  <si>
+    <t>C-106786</t>
+  </si>
+  <si>
+    <t>10-1307989</t>
+  </si>
+  <si>
+    <t>C-106787</t>
+  </si>
+  <si>
+    <t>10-1307992</t>
+  </si>
+  <si>
+    <t>C-106788</t>
+  </si>
+  <si>
+    <t>10-1308042</t>
+  </si>
+  <si>
+    <t>C-106789</t>
+  </si>
+  <si>
+    <t>10-1308155</t>
+  </si>
+  <si>
+    <t>C-106818</t>
+  </si>
+  <si>
+    <t>10-1308156</t>
+  </si>
+  <si>
+    <t>C-106819</t>
+  </si>
+  <si>
+    <t>10-1308158</t>
+  </si>
+  <si>
+    <t>C-106820</t>
+  </si>
+  <si>
+    <t>10-1308161</t>
+  </si>
+  <si>
+    <t>C-106826</t>
+  </si>
+  <si>
+    <t>10-1308164</t>
+  </si>
+  <si>
+    <t>C-106828</t>
+  </si>
+  <si>
+    <t>10-1308165</t>
+  </si>
+  <si>
+    <t>C-106829</t>
+  </si>
+  <si>
+    <t>10-1308167</t>
+  </si>
+  <si>
+    <t>C-106831</t>
+  </si>
+  <si>
+    <t>10-1308168</t>
+  </si>
+  <si>
+    <t>C-106832</t>
   </si>
 </sst>
 </file>
@@ -2875,10 +3106,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C429"/>
+  <dimension ref="A1:C470"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A409" workbookViewId="0">
-      <selection activeCell="A429" sqref="A429"/>
+    <sheetView tabSelected="1" topLeftCell="A454" workbookViewId="0">
+      <selection activeCell="A470" sqref="A470"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5064,6 +5295,211 @@
         <v>802</v>
       </c>
     </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A433" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A435" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A436" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A437" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A438" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A439" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A441" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A453" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A454" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A456" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A457" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A459" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A461" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A463" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A464" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>879</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
@@ -5072,10 +5508,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:C371"/>
+  <dimension ref="A2:C409"/>
   <sheetViews>
-    <sheetView topLeftCell="A339" workbookViewId="0">
-      <selection activeCell="A351" sqref="A351"/>
+    <sheetView topLeftCell="A381" workbookViewId="0">
+      <selection activeCell="A390" sqref="A390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6938,9 +7374,199 @@
         <v>801</v>
       </c>
     </row>
-    <row r="371">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>803</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A399" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A400" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="s">
+        <v>880</v>
       </c>
     </row>
   </sheetData>

</xml_diff>